<commit_message>
added route function for read file
</commit_message>
<xml_diff>
--- a/forecast_pivot.xlsx
+++ b/forecast_pivot.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,286 +436,592 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>S.No</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Client Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>PO No</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2025-05</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>2025-07</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-08</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-09</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-10</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-11</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-12</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2026-01</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2026-02</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2026-03</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2026-04</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2026-05</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2026-06</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2026-07</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2026-08</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2026-09</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2026-10</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Fiona Inc</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1234567345</t>
-        </is>
-      </c>
       <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
+        <v>34523</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>$16,000.00</t>
+        </is>
       </c>
       <c r="E2" t="n">
-        <v>5333.333333333333</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>5333.333333333333</v>
-      </c>
-      <c r="G2" t="n">
-        <v>5333.333333333333</v>
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>$32,000.00</t>
+        </is>
       </c>
       <c r="H2" t="n">
-        <v>5333.333333333333</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>5333.333333333333</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>5333.333333333333</v>
-      </c>
-      <c r="K2" t="n">
-        <v>5333.333333333333</v>
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>$32,000.00</t>
+        </is>
       </c>
       <c r="L2" t="n">
-        <v>5333.333333333333</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>5333.333333333333</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>5333.333333333333</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>5333.333333333333</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>5333.333333333333</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>5333.333333333333</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>5333.333333333333</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>5333.333333333333</v>
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Fiona Inc</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1234567890</t>
-        </is>
-      </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1234567345</v>
       </c>
       <c r="D3" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F3" t="n">
-        <v>10000</v>
-      </c>
-      <c r="G3" t="n">
-        <v>15000</v>
-      </c>
-      <c r="H3" t="n">
-        <v>15000</v>
-      </c>
-      <c r="I3" t="n">
-        <v>10000</v>
-      </c>
-      <c r="J3" t="n">
-        <v>10000</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Fiona Inc</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>$10,000.00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>$10,000.00</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>$10,000.00</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>$15,000.00</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>$15,000.00</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>$10,000.00</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>$10,000.00</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Fiona Inc</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1234567345</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Fiona Inc</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>$10,000.00</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>$10,000.00</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>$10,000.00</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>$15,000.00</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>$15,000.00</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>$10,000.00</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>$10,000.00</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Fiona Inc</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>34523</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>16000</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>32000</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>32000</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" t="n">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$16,000.00</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>$32,000.00</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>$32,000.00</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
small fix with consistency in forecast output
</commit_message>
<xml_diff>
--- a/forecast_pivot.xlsx
+++ b/forecast_pivot.xlsx
@@ -55,11 +55,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -554,58 +555,58 @@
           <t>1234567345</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>5333.33</v>
-      </c>
-      <c r="H2" t="n">
-        <v>5333.33</v>
-      </c>
-      <c r="I2" t="n">
-        <v>5333.33</v>
-      </c>
-      <c r="J2" t="n">
-        <v>5333.33</v>
-      </c>
-      <c r="K2" t="n">
-        <v>5333.33</v>
-      </c>
-      <c r="L2" t="n">
-        <v>5333.33</v>
-      </c>
-      <c r="M2" t="n">
-        <v>5333.33</v>
-      </c>
-      <c r="N2" t="n">
-        <v>5333.33</v>
-      </c>
-      <c r="O2" t="n">
-        <v>5333.33</v>
-      </c>
-      <c r="P2" t="n">
-        <v>5333.33</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>5333.33</v>
-      </c>
-      <c r="R2" t="n">
-        <v>5333.33</v>
-      </c>
-      <c r="S2" t="n">
-        <v>5333.33</v>
-      </c>
-      <c r="T2" t="n">
-        <v>5333.33</v>
-      </c>
-      <c r="U2" t="n">
+      <c r="D2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="U2" s="2" t="n">
         <v>5333.33</v>
       </c>
     </row>
@@ -623,58 +624,58 @@
           <t>1234567890</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <v>10000</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" s="2" t="n">
         <v>10000</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" s="2" t="n">
         <v>10000</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" s="2" t="n">
         <v>15000</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J3" s="2" t="n">
         <v>15000</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K3" s="2" t="n">
         <v>10000</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L3" s="2" t="n">
         <v>10000</v>
       </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" t="n">
+      <c r="M3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -692,58 +693,58 @@
           <t>34523</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="2" t="n">
         <v>16000</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
+      <c r="E4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="n">
         <v>32000</v>
       </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
+      <c r="I4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2" t="n">
         <v>32000</v>
       </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" t="n">
+      <c r="M4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
templates and auth added
</commit_message>
<xml_diff>
--- a/forecast_pivot.xlsx
+++ b/forecast_pivot.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,65 +544,91 @@
           <t>Fiona Inc</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>34523</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>$16,000.00</t>
-        </is>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1234567345</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>$32,000.00</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>$32,000.00</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0</v>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>$5,333.33</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -614,89 +640,75 @@
           <t>Fiona Inc</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>1234567345</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="E3" t="n">
-        <v>0</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>$10,000.00</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>$5,333.33</t>
+          <t>$10,000.00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>$5,333.33</t>
+          <t>$10,000.00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>$5,333.33</t>
+          <t>$15,000.00</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>$5,333.33</t>
+          <t>$15,000.00</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>$5,333.33</t>
+          <t>$10,000.00</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
+          <t>$10,000.00</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -708,45 +720,39 @@
           <t>Fiona Inc</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>1234567890</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>$10,000.00</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>$10,000.00</t>
-        </is>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>34523</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>$16,000.00</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>$10,000.00</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>$15,000.00</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>$15,000.00</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>$10,000.00</t>
-        </is>
+          <t>$32,000.00</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>$10,000.00</t>
+          <t>$32,000.00</t>
         </is>
       </c>
       <c r="L4" t="n">
@@ -774,254 +780,6 @@
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Fiona Inc</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1234567345</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>$5,333.33</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Fiona Inc</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>1234567890</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>$10,000.00</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>$10,000.00</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>$10,000.00</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>$15,000.00</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>$15,000.00</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>$10,000.00</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>$10,000.00</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Fiona Inc</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>34523</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>$16,000.00</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>$32,000.00</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>$32,000.00</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0</v>
-      </c>
-      <c r="T7" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
project owner filter to the pivot table
</commit_message>
<xml_diff>
--- a/forecast_pivot.xlsx
+++ b/forecast_pivot.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,90 +452,95 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Project Owner</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>2025-05</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2025-06</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>2025-07</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>2025-08</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>2025-09</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>2025-10</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2025-11</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>2025-12</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>2026-01</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>2026-02</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>2026-03</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>2026-04</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2026-05</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>2026-06</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>2026-07</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>2026-08</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>2026-09</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>2026-10</t>
         </is>
@@ -555,8 +560,10 @@
           <t>1234567345</t>
         </is>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>0</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ProjectOwner2</t>
+        </is>
       </c>
       <c r="E2" s="2" t="n">
         <v>0</v>
@@ -565,7 +572,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>5333.33</v>
+        <v>0</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>5333.33</v>
@@ -607,6 +614,9 @@
         <v>5333.33</v>
       </c>
       <c r="U2" s="2" t="n">
+        <v>5333.33</v>
+      </c>
+      <c r="V2" s="2" t="n">
         <v>5333.33</v>
       </c>
     </row>
@@ -624,14 +634,16 @@
           <t>1234567890</t>
         </is>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>0</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ProjectOwner2</t>
+        </is>
       </c>
       <c r="E3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>10000</v>
@@ -640,19 +652,19 @@
         <v>10000</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="J3" s="2" t="n">
         <v>15000</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="L3" s="2" t="n">
         <v>10000</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="N3" s="2" t="n">
         <v>0</v>
@@ -676,6 +688,9 @@
         <v>0</v>
       </c>
       <c r="U3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -693,12 +708,14 @@
           <t>34523</t>
         </is>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ProjectOwner1</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="n">
         <v>16000</v>
       </c>
-      <c r="E4" s="2" t="n">
-        <v>0</v>
-      </c>
       <c r="F4" s="2" t="n">
         <v>0</v>
       </c>
@@ -706,11 +723,11 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="n">
         <v>32000</v>
       </c>
-      <c r="I4" s="2" t="n">
-        <v>0</v>
-      </c>
       <c r="J4" s="2" t="n">
         <v>0</v>
       </c>
@@ -718,11 +735,11 @@
         <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2" t="n">
         <v>32000</v>
       </c>
-      <c r="M4" s="2" t="n">
-        <v>0</v>
-      </c>
       <c r="N4" s="2" t="n">
         <v>0</v>
       </c>
@@ -745,6 +762,9 @@
         <v>0</v>
       </c>
       <c r="U4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new form updated
</commit_message>
<xml_diff>
--- a/forecast_pivot.xlsx
+++ b/forecast_pivot.xlsx
@@ -562,7 +562,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ProjectOwner2</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
@@ -575,49 +575,49 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
       <c r="R2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
       <c r="S2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
       <c r="U2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
       <c r="V2" s="2" t="n">
-        <v>10000</v>
+        <v>5333.33</v>
       </c>
     </row>
     <row r="3">
@@ -636,7 +636,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ProjectOwner2</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E3" s="2" t="n">
@@ -710,11 +710,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ProjectOwner1</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>20000</v>
+        <v>16000</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0</v>
@@ -726,7 +726,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>40000</v>
+        <v>32000</v>
       </c>
       <c r="J4" s="2" t="n">
         <v>0</v>
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>40000</v>
+        <v>32000</v>
       </c>
       <c r="N4" s="2" t="n">
         <v>0</v>

</xml_diff>